<commit_message>
Refactor some js files
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -396,10 +396,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,11 +750,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -773,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Add edit profile form
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,7 +888,9 @@
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5">
+        <v>3</v>
+      </c>
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1208,7 +1210,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>